<commit_message>
One Signup test case
</commit_message>
<xml_diff>
--- a/resources/locators.xlsx
+++ b/resources/locators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaNi569\Desktop\CRMUIA\Generic_web_automation_framework\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334063A1-1D43-4F4F-A853-BFC931CED48B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621B3382-6640-416B-94A2-A004AC0C8EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5EBB3FE3-55C9-4B90-8FD4-935120834B2F}"/>
+    <workbookView xWindow="32505" yWindow="1755" windowWidth="19185" windowHeight="10065" xr2:uid="{5EBB3FE3-55C9-4B90-8FD4-935120834B2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="80">
   <si>
     <t>Page</t>
   </si>
@@ -237,6 +237,45 @@
   </si>
   <si>
     <t>//div[@class='mat-mdc-snack-bar-label mdc-snackbar__label']</t>
+  </si>
+  <si>
+    <t>SignupPage</t>
+  </si>
+  <si>
+    <t>Signup Link</t>
+  </si>
+  <si>
+    <t>//a[@routerlink='/auth/register']</t>
+  </si>
+  <si>
+    <t>Signup button</t>
+  </si>
+  <si>
+    <t>//input[@formcontrolname='termsCheck']</t>
+  </si>
+  <si>
+    <t>Terms Checkbox</t>
+  </si>
+  <si>
+    <t>Plan Premium</t>
+  </si>
+  <si>
+    <t>//label/span[normalize-space()='Premium']</t>
+  </si>
+  <si>
+    <t>//input[@formcontrolname='UserName']</t>
+  </si>
+  <si>
+    <t>//input[@formcontrolname='CompanyName']</t>
+  </si>
+  <si>
+    <t>//input[@formcontrolname='Email']</t>
+  </si>
+  <si>
+    <t>(//mat-option[@id='mat-option-350'])[1]</t>
+  </si>
+  <si>
+    <t>//input[@formcontrolname='PhoneNumber']</t>
   </si>
 </sst>
 </file>
@@ -313,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -330,6 +369,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -665,16 +716,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41983873-4B55-4713-B31B-EDCB84D265C4}">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:D111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.453125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="32.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.81640625" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="65.1796875" style="1" bestFit="1" customWidth="1"/>
   </cols>
@@ -683,7 +734,7 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -693,999 +744,1125 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>5</v>
+        <v>67</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D2" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>7</v>
+        <v>67</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D3" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>67</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>22</v>
+        <v>4</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>23</v>
+      <c r="D11" s="8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>24</v>
+        <v>4</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>25</v>
+      <c r="D12" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>26</v>
+        <v>4</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>27</v>
+      <c r="D13" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>28</v>
+        <v>4</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>29</v>
+      <c r="D14" s="8" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>30</v>
+      <c r="B15" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="D15" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>32</v>
+      <c r="B16" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>33</v>
+      <c r="D16" s="8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>34</v>
+      <c r="B17" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>35</v>
+      <c r="D17" s="8" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>36</v>
+      <c r="B18" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D18" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>38</v>
+      <c r="B19" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>39</v>
+      <c r="D19" s="8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>40</v>
+      <c r="B20" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>41</v>
+      <c r="D20" s="8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>42</v>
+      <c r="B21" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>43</v>
+      <c r="D21" s="8" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>44</v>
+      <c r="B22" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>45</v>
+      <c r="D22" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>46</v>
+      <c r="B23" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>47</v>
+      <c r="D23" s="8" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>48</v>
+      <c r="B24" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D24" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>50</v>
+      <c r="B25" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="D25" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>52</v>
+      <c r="B26" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>53</v>
+      <c r="D26" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>54</v>
+      <c r="B27" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="D27" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>56</v>
+      <c r="B28" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="D28" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>58</v>
+      <c r="B29" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>59</v>
+      <c r="D29" s="8" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>60</v>
+      <c r="B30" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>61</v>
+      <c r="D30" s="8" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>62</v>
+      <c r="B31" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>63</v>
+      <c r="D31" s="8" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="A35" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="A37" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="A38" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="5" t="s">
+      <c r="C41" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="6">
-        <v>31</v>
-      </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-    </row>
-    <row r="34" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="6">
-        <v>32</v>
-      </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-    </row>
-    <row r="35" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="6">
-        <v>33</v>
-      </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-    </row>
-    <row r="36" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="6">
-        <v>34</v>
-      </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-    </row>
-    <row r="37" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="6">
-        <v>35</v>
-      </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-    </row>
-    <row r="38" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="6">
-        <v>36</v>
-      </c>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-    </row>
-    <row r="39" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="6">
-        <v>37</v>
-      </c>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-    </row>
-    <row r="40" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="6">
-        <v>38</v>
-      </c>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-    </row>
-    <row r="41" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="6">
-        <v>39</v>
-      </c>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
     </row>
     <row r="42" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A42" s="6">
-        <v>40</v>
-      </c>
-      <c r="B42" s="6"/>
+        <v>31</v>
+      </c>
+      <c r="B42" s="9"/>
       <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
+      <c r="D42" s="9"/>
     </row>
     <row r="43" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="6">
-        <v>41</v>
-      </c>
-      <c r="B43" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="B43" s="9"/>
       <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
+      <c r="D43" s="9"/>
     </row>
     <row r="44" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="6">
-        <v>42</v>
-      </c>
-      <c r="B44" s="6"/>
+        <v>33</v>
+      </c>
+      <c r="B44" s="9"/>
       <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
+      <c r="D44" s="9"/>
     </row>
     <row r="45" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A45" s="6">
-        <v>43</v>
-      </c>
-      <c r="B45" s="6"/>
+        <v>34</v>
+      </c>
+      <c r="B45" s="9"/>
       <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
+      <c r="D45" s="9"/>
     </row>
     <row r="46" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A46" s="6">
-        <v>44</v>
-      </c>
-      <c r="B46" s="6"/>
+        <v>35</v>
+      </c>
+      <c r="B46" s="9"/>
       <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
+      <c r="D46" s="9"/>
     </row>
     <row r="47" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A47" s="6">
-        <v>45</v>
-      </c>
-      <c r="B47" s="6"/>
+        <v>36</v>
+      </c>
+      <c r="B47" s="9"/>
       <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
+      <c r="D47" s="9"/>
     </row>
     <row r="48" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A48" s="6">
-        <v>46</v>
-      </c>
-      <c r="B48" s="6"/>
+        <v>37</v>
+      </c>
+      <c r="B48" s="9"/>
       <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
+      <c r="D48" s="9"/>
     </row>
     <row r="49" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A49" s="6">
-        <v>47</v>
-      </c>
-      <c r="B49" s="6"/>
+        <v>38</v>
+      </c>
+      <c r="B49" s="9"/>
       <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
+      <c r="D49" s="9"/>
     </row>
     <row r="50" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A50" s="6">
-        <v>48</v>
-      </c>
-      <c r="B50" s="6"/>
+        <v>39</v>
+      </c>
+      <c r="B50" s="9"/>
       <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
+      <c r="D50" s="9"/>
     </row>
     <row r="51" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A51" s="6">
-        <v>49</v>
-      </c>
-      <c r="B51" s="6"/>
+        <v>40</v>
+      </c>
+      <c r="B51" s="9"/>
       <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
+      <c r="D51" s="9"/>
     </row>
     <row r="52" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A52" s="6">
-        <v>50</v>
-      </c>
-      <c r="B52" s="6"/>
+        <v>41</v>
+      </c>
+      <c r="B52" s="9"/>
       <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
+      <c r="D52" s="9"/>
     </row>
     <row r="53" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A53" s="6">
-        <v>51</v>
-      </c>
-      <c r="B53" s="6"/>
+        <v>42</v>
+      </c>
+      <c r="B53" s="9"/>
       <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
+      <c r="D53" s="9"/>
     </row>
     <row r="54" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A54" s="6">
-        <v>52</v>
-      </c>
-      <c r="B54" s="6"/>
+        <v>43</v>
+      </c>
+      <c r="B54" s="9"/>
       <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
+      <c r="D54" s="9"/>
     </row>
     <row r="55" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A55" s="6">
-        <v>53</v>
-      </c>
-      <c r="B55" s="6"/>
+        <v>44</v>
+      </c>
+      <c r="B55" s="9"/>
       <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
+      <c r="D55" s="9"/>
     </row>
     <row r="56" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A56" s="6">
-        <v>54</v>
-      </c>
-      <c r="B56" s="6"/>
+        <v>45</v>
+      </c>
+      <c r="B56" s="9"/>
       <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
+      <c r="D56" s="9"/>
     </row>
     <row r="57" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A57" s="6">
-        <v>55</v>
-      </c>
-      <c r="B57" s="6"/>
+        <v>46</v>
+      </c>
+      <c r="B57" s="9"/>
       <c r="C57" s="6"/>
-      <c r="D57" s="6"/>
+      <c r="D57" s="9"/>
     </row>
     <row r="58" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A58" s="6">
-        <v>56</v>
-      </c>
-      <c r="B58" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="B58" s="9"/>
       <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
+      <c r="D58" s="9"/>
     </row>
     <row r="59" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A59" s="6">
-        <v>57</v>
-      </c>
-      <c r="B59" s="6"/>
+        <v>48</v>
+      </c>
+      <c r="B59" s="9"/>
       <c r="C59" s="6"/>
-      <c r="D59" s="6"/>
+      <c r="D59" s="9"/>
     </row>
     <row r="60" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A60" s="6">
-        <v>58</v>
-      </c>
-      <c r="B60" s="6"/>
+        <v>49</v>
+      </c>
+      <c r="B60" s="9"/>
       <c r="C60" s="6"/>
-      <c r="D60" s="6"/>
+      <c r="D60" s="9"/>
     </row>
     <row r="61" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A61" s="6">
-        <v>59</v>
-      </c>
-      <c r="B61" s="6"/>
+        <v>50</v>
+      </c>
+      <c r="B61" s="9"/>
       <c r="C61" s="6"/>
-      <c r="D61" s="6"/>
+      <c r="D61" s="9"/>
     </row>
     <row r="62" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A62" s="6">
-        <v>60</v>
-      </c>
-      <c r="B62" s="6"/>
+        <v>51</v>
+      </c>
+      <c r="B62" s="9"/>
       <c r="C62" s="6"/>
-      <c r="D62" s="6"/>
+      <c r="D62" s="9"/>
     </row>
     <row r="63" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A63" s="6">
-        <v>61</v>
-      </c>
-      <c r="B63" s="6"/>
+        <v>52</v>
+      </c>
+      <c r="B63" s="9"/>
       <c r="C63" s="6"/>
-      <c r="D63" s="6"/>
+      <c r="D63" s="9"/>
     </row>
     <row r="64" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A64" s="6">
-        <v>62</v>
-      </c>
-      <c r="B64" s="6"/>
+        <v>53</v>
+      </c>
+      <c r="B64" s="9"/>
       <c r="C64" s="6"/>
-      <c r="D64" s="6"/>
+      <c r="D64" s="9"/>
     </row>
     <row r="65" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A65" s="6">
-        <v>63</v>
-      </c>
-      <c r="B65" s="6"/>
+        <v>54</v>
+      </c>
+      <c r="B65" s="9"/>
       <c r="C65" s="6"/>
-      <c r="D65" s="6"/>
+      <c r="D65" s="9"/>
     </row>
     <row r="66" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A66" s="6">
-        <v>64</v>
-      </c>
-      <c r="B66" s="6"/>
+        <v>55</v>
+      </c>
+      <c r="B66" s="9"/>
       <c r="C66" s="6"/>
-      <c r="D66" s="6"/>
+      <c r="D66" s="9"/>
     </row>
     <row r="67" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A67" s="6">
-        <v>65</v>
-      </c>
-      <c r="B67" s="6"/>
+        <v>56</v>
+      </c>
+      <c r="B67" s="9"/>
       <c r="C67" s="6"/>
       <c r="D67" s="6"/>
     </row>
     <row r="68" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A68" s="6">
-        <v>66</v>
-      </c>
-      <c r="B68" s="6"/>
+        <v>57</v>
+      </c>
+      <c r="B68" s="9"/>
       <c r="C68" s="6"/>
       <c r="D68" s="6"/>
     </row>
     <row r="69" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A69" s="6">
-        <v>67</v>
-      </c>
-      <c r="B69" s="6"/>
+        <v>58</v>
+      </c>
+      <c r="B69" s="9"/>
       <c r="C69" s="6"/>
       <c r="D69" s="6"/>
     </row>
     <row r="70" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A70" s="6">
-        <v>68</v>
-      </c>
-      <c r="B70" s="6"/>
+        <v>59</v>
+      </c>
+      <c r="B70" s="9"/>
       <c r="C70" s="6"/>
       <c r="D70" s="6"/>
     </row>
     <row r="71" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A71" s="6">
-        <v>69</v>
-      </c>
-      <c r="B71" s="6"/>
+        <v>60</v>
+      </c>
+      <c r="B71" s="9"/>
       <c r="C71" s="6"/>
       <c r="D71" s="6"/>
     </row>
     <row r="72" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A72" s="6">
-        <v>70</v>
-      </c>
-      <c r="B72" s="6"/>
+        <v>61</v>
+      </c>
+      <c r="B72" s="9"/>
       <c r="C72" s="6"/>
       <c r="D72" s="6"/>
     </row>
     <row r="73" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A73" s="6">
-        <v>71</v>
-      </c>
-      <c r="B73" s="6"/>
+        <v>62</v>
+      </c>
+      <c r="B73" s="9"/>
       <c r="C73" s="6"/>
       <c r="D73" s="6"/>
     </row>
     <row r="74" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A74" s="6">
-        <v>72</v>
-      </c>
-      <c r="B74" s="6"/>
+        <v>63</v>
+      </c>
+      <c r="B74" s="9"/>
       <c r="C74" s="6"/>
       <c r="D74" s="6"/>
     </row>
     <row r="75" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A75" s="6">
-        <v>73</v>
-      </c>
-      <c r="B75" s="6"/>
+        <v>64</v>
+      </c>
+      <c r="B75" s="9"/>
       <c r="C75" s="6"/>
       <c r="D75" s="6"/>
     </row>
     <row r="76" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A76" s="6">
-        <v>74</v>
-      </c>
-      <c r="B76" s="6"/>
+        <v>65</v>
+      </c>
+      <c r="B76" s="9"/>
       <c r="C76" s="6"/>
       <c r="D76" s="6"/>
     </row>
     <row r="77" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A77" s="6">
-        <v>75</v>
-      </c>
-      <c r="B77" s="6"/>
+        <v>66</v>
+      </c>
+      <c r="B77" s="9"/>
       <c r="C77" s="6"/>
       <c r="D77" s="6"/>
     </row>
     <row r="78" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A78" s="6">
-        <v>76</v>
-      </c>
-      <c r="B78" s="6"/>
+        <v>67</v>
+      </c>
+      <c r="B78" s="9"/>
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
     </row>
     <row r="79" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A79" s="6">
-        <v>77</v>
-      </c>
-      <c r="B79" s="6"/>
+        <v>68</v>
+      </c>
+      <c r="B79" s="9"/>
       <c r="C79" s="6"/>
       <c r="D79" s="6"/>
     </row>
     <row r="80" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A80" s="6">
-        <v>78</v>
-      </c>
-      <c r="B80" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="B80" s="9"/>
       <c r="C80" s="6"/>
       <c r="D80" s="6"/>
     </row>
     <row r="81" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A81" s="6">
-        <v>79</v>
-      </c>
-      <c r="B81" s="6"/>
+        <v>70</v>
+      </c>
+      <c r="B81" s="9"/>
       <c r="C81" s="6"/>
       <c r="D81" s="6"/>
     </row>
     <row r="82" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A82" s="6">
-        <v>80</v>
-      </c>
-      <c r="B82" s="6"/>
+        <v>71</v>
+      </c>
+      <c r="B82" s="9"/>
       <c r="C82" s="6"/>
       <c r="D82" s="6"/>
     </row>
     <row r="83" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A83" s="6">
-        <v>81</v>
-      </c>
-      <c r="B83" s="6"/>
+        <v>72</v>
+      </c>
+      <c r="B83" s="9"/>
       <c r="C83" s="6"/>
       <c r="D83" s="6"/>
     </row>
     <row r="84" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A84" s="6">
-        <v>82</v>
-      </c>
-      <c r="B84" s="6"/>
+        <v>73</v>
+      </c>
+      <c r="B84" s="9"/>
       <c r="C84" s="6"/>
       <c r="D84" s="6"/>
     </row>
     <row r="85" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A85" s="6">
-        <v>83</v>
-      </c>
-      <c r="B85" s="6"/>
+        <v>74</v>
+      </c>
+      <c r="B85" s="9"/>
       <c r="C85" s="6"/>
       <c r="D85" s="6"/>
     </row>
     <row r="86" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A86" s="6">
-        <v>84</v>
-      </c>
-      <c r="B86" s="6"/>
+        <v>75</v>
+      </c>
+      <c r="B86" s="9"/>
       <c r="C86" s="6"/>
       <c r="D86" s="6"/>
     </row>
     <row r="87" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A87" s="6">
-        <v>85</v>
-      </c>
-      <c r="B87" s="6"/>
+        <v>76</v>
+      </c>
+      <c r="B87" s="9"/>
       <c r="C87" s="6"/>
       <c r="D87" s="6"/>
     </row>
     <row r="88" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A88" s="6">
-        <v>86</v>
-      </c>
-      <c r="B88" s="6"/>
+        <v>77</v>
+      </c>
+      <c r="B88" s="9"/>
       <c r="C88" s="6"/>
       <c r="D88" s="6"/>
     </row>
     <row r="89" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A89" s="6">
-        <v>87</v>
-      </c>
-      <c r="B89" s="6"/>
+        <v>78</v>
+      </c>
+      <c r="B89" s="9"/>
       <c r="C89" s="6"/>
       <c r="D89" s="6"/>
     </row>
     <row r="90" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A90" s="6">
-        <v>88</v>
-      </c>
-      <c r="B90" s="6"/>
+        <v>79</v>
+      </c>
+      <c r="B90" s="9"/>
       <c r="C90" s="6"/>
       <c r="D90" s="6"/>
     </row>
     <row r="91" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A91" s="6">
-        <v>89</v>
-      </c>
-      <c r="B91" s="6"/>
+        <v>80</v>
+      </c>
+      <c r="B91" s="9"/>
       <c r="C91" s="6"/>
       <c r="D91" s="6"/>
     </row>
     <row r="92" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A92" s="6">
-        <v>90</v>
-      </c>
-      <c r="B92" s="6"/>
+        <v>81</v>
+      </c>
+      <c r="B92" s="9"/>
       <c r="C92" s="6"/>
       <c r="D92" s="6"/>
     </row>
     <row r="93" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A93" s="6">
-        <v>91</v>
-      </c>
-      <c r="B93" s="6"/>
+        <v>82</v>
+      </c>
+      <c r="B93" s="9"/>
       <c r="C93" s="6"/>
       <c r="D93" s="6"/>
     </row>
     <row r="94" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A94" s="6">
-        <v>92</v>
-      </c>
-      <c r="B94" s="6"/>
+        <v>83</v>
+      </c>
+      <c r="B94" s="9"/>
       <c r="C94" s="6"/>
       <c r="D94" s="6"/>
     </row>
     <row r="95" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A95" s="6">
-        <v>93</v>
-      </c>
-      <c r="B95" s="6"/>
+        <v>84</v>
+      </c>
+      <c r="B95" s="9"/>
       <c r="C95" s="6"/>
       <c r="D95" s="6"/>
     </row>
     <row r="96" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A96" s="6">
-        <v>94</v>
-      </c>
-      <c r="B96" s="6"/>
+        <v>85</v>
+      </c>
+      <c r="B96" s="9"/>
       <c r="C96" s="6"/>
       <c r="D96" s="6"/>
     </row>
     <row r="97" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A97" s="6">
-        <v>95</v>
-      </c>
-      <c r="B97" s="6"/>
+        <v>86</v>
+      </c>
+      <c r="B97" s="9"/>
       <c r="C97" s="6"/>
       <c r="D97" s="6"/>
     </row>
     <row r="98" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A98" s="6">
-        <v>96</v>
-      </c>
-      <c r="B98" s="6"/>
+        <v>87</v>
+      </c>
+      <c r="B98" s="9"/>
       <c r="C98" s="6"/>
       <c r="D98" s="6"/>
     </row>
     <row r="99" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A99" s="6">
-        <v>97</v>
-      </c>
-      <c r="B99" s="6"/>
+        <v>88</v>
+      </c>
+      <c r="B99" s="9"/>
       <c r="C99" s="6"/>
       <c r="D99" s="6"/>
     </row>
     <row r="100" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A100" s="6">
-        <v>98</v>
-      </c>
-      <c r="B100" s="6"/>
+        <v>89</v>
+      </c>
+      <c r="B100" s="9"/>
       <c r="C100" s="6"/>
       <c r="D100" s="6"/>
     </row>
     <row r="101" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A101" s="6">
-        <v>99</v>
-      </c>
-      <c r="B101" s="6"/>
+        <v>90</v>
+      </c>
+      <c r="B101" s="9"/>
       <c r="C101" s="6"/>
       <c r="D101" s="6"/>
     </row>
     <row r="102" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A102" s="6">
-        <v>100</v>
-      </c>
-      <c r="B102" s="6"/>
+        <v>91</v>
+      </c>
+      <c r="B102" s="9"/>
       <c r="C102" s="6"/>
       <c r="D102" s="6"/>
+    </row>
+    <row r="103" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A103" s="6">
+        <v>92</v>
+      </c>
+      <c r="B103" s="9"/>
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
+    </row>
+    <row r="104" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A104" s="6">
+        <v>93</v>
+      </c>
+      <c r="B104" s="9"/>
+      <c r="C104" s="6"/>
+      <c r="D104" s="6"/>
+    </row>
+    <row r="105" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A105" s="6">
+        <v>94</v>
+      </c>
+      <c r="B105" s="9"/>
+      <c r="C105" s="6"/>
+      <c r="D105" s="6"/>
+    </row>
+    <row r="106" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A106" s="6">
+        <v>95</v>
+      </c>
+      <c r="B106" s="9"/>
+      <c r="C106" s="6"/>
+      <c r="D106" s="6"/>
+    </row>
+    <row r="107" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A107" s="6">
+        <v>96</v>
+      </c>
+      <c r="B107" s="9"/>
+      <c r="C107" s="6"/>
+      <c r="D107" s="6"/>
+    </row>
+    <row r="108" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A108" s="6">
+        <v>97</v>
+      </c>
+      <c r="B108" s="9"/>
+      <c r="C108" s="6"/>
+      <c r="D108" s="6"/>
+    </row>
+    <row r="109" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A109" s="6">
+        <v>98</v>
+      </c>
+      <c r="B109" s="9"/>
+      <c r="C109" s="6"/>
+      <c r="D109" s="6"/>
+    </row>
+    <row r="110" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A110" s="6">
+        <v>99</v>
+      </c>
+      <c r="B110" s="9"/>
+      <c r="C110" s="6"/>
+      <c r="D110" s="6"/>
+    </row>
+    <row r="111" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A111" s="6">
+        <v>100</v>
+      </c>
+      <c r="B111" s="9"/>
+      <c r="C111" s="6"/>
+      <c r="D111" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
One Signup test case error fixed
</commit_message>
<xml_diff>
--- a/resources/locators.xlsx
+++ b/resources/locators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaNi569\Desktop\CRMUIA\Generic_web_automation_framework\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621B3382-6640-416B-94A2-A004AC0C8EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C1E6B2-3173-4689-AE84-7B69F4F14F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32505" yWindow="1755" windowWidth="19185" windowHeight="10065" xr2:uid="{5EBB3FE3-55C9-4B90-8FD4-935120834B2F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="82">
   <si>
     <t>Page</t>
   </si>
@@ -248,9 +248,6 @@
     <t>//a[@routerlink='/auth/register']</t>
   </si>
   <si>
-    <t>Signup button</t>
-  </si>
-  <si>
     <t>//input[@formcontrolname='termsCheck']</t>
   </si>
   <si>
@@ -276,6 +273,15 @@
   </si>
   <si>
     <t>//input[@formcontrolname='PhoneNumber']</t>
+  </si>
+  <si>
+    <t>//span[@class='mdc-button__label']</t>
+  </si>
+  <si>
+    <t>Success Message</t>
+  </si>
+  <si>
+    <t>Signup Button</t>
   </si>
 </sst>
 </file>
@@ -716,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41983873-4B55-4713-B31B-EDCB84D265C4}">
-  <dimension ref="A1:D111"/>
+  <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -769,7 +775,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
@@ -783,7 +789,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
@@ -797,7 +803,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
@@ -811,7 +817,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
@@ -825,7 +831,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
@@ -833,13 +839,13 @@
         <v>67</v>
       </c>
       <c r="B8" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>73</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
@@ -847,13 +853,13 @@
         <v>67</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
@@ -861,7 +867,7 @@
         <v>67</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>6</v>
@@ -870,32 +876,32 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>5</v>
+        <v>67</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D11" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>10</v>
+      <c r="D12" s="9" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -903,13 +909,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -917,41 +923,41 @@
         <v>4</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -959,13 +965,13 @@
         <v>12</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -973,27 +979,27 @@
         <v>12</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -1001,27 +1007,27 @@
         <v>12</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -1029,13 +1035,13 @@
         <v>12</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -1043,13 +1049,13 @@
         <v>12</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -1057,27 +1063,27 @@
         <v>12</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -1085,27 +1091,27 @@
         <v>12</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -1113,13 +1119,13 @@
         <v>12</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -1127,13 +1133,13 @@
         <v>12</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -1141,13 +1147,13 @@
         <v>12</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -1155,13 +1161,13 @@
         <v>12</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -1169,13 +1175,13 @@
         <v>12</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -1183,13 +1189,13 @@
         <v>12</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -1197,27 +1203,27 @@
         <v>12</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -1225,13 +1231,13 @@
         <v>12</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="31" x14ac:dyDescent="0.35">
@@ -1239,55 +1245,55 @@
         <v>12</v>
       </c>
       <c r="B37" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="A39" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="8" t="s">
+      <c r="C39" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A38" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B38" s="8" t="s">
+    <row r="40" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="A40" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C38" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="8" t="s">
+      <c r="C40" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="8" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -1295,34 +1301,46 @@
         <v>12</v>
       </c>
       <c r="B41" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A43" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C41" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" s="8" t="s">
+      <c r="C43" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="6">
-        <v>31</v>
-      </c>
-      <c r="B42" s="9"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="9"/>
-    </row>
-    <row r="43" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="6">
-        <v>32</v>
-      </c>
-      <c r="B43" s="9"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="9"/>
     </row>
     <row r="44" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="6">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="6"/>
@@ -1330,7 +1348,7 @@
     </row>
     <row r="45" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A45" s="6">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B45" s="9"/>
       <c r="C45" s="6"/>
@@ -1338,7 +1356,7 @@
     </row>
     <row r="46" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A46" s="6">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B46" s="9"/>
       <c r="C46" s="6"/>
@@ -1346,7 +1364,7 @@
     </row>
     <row r="47" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A47" s="6">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B47" s="9"/>
       <c r="C47" s="6"/>
@@ -1354,7 +1372,7 @@
     </row>
     <row r="48" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A48" s="6">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B48" s="9"/>
       <c r="C48" s="6"/>
@@ -1362,7 +1380,7 @@
     </row>
     <row r="49" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A49" s="6">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B49" s="9"/>
       <c r="C49" s="6"/>
@@ -1370,7 +1388,7 @@
     </row>
     <row r="50" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A50" s="6">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B50" s="9"/>
       <c r="C50" s="6"/>
@@ -1378,7 +1396,7 @@
     </row>
     <row r="51" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A51" s="6">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B51" s="9"/>
       <c r="C51" s="6"/>
@@ -1386,7 +1404,7 @@
     </row>
     <row r="52" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A52" s="6">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B52" s="9"/>
       <c r="C52" s="6"/>
@@ -1394,7 +1412,7 @@
     </row>
     <row r="53" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A53" s="6">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B53" s="9"/>
       <c r="C53" s="6"/>
@@ -1402,7 +1420,7 @@
     </row>
     <row r="54" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A54" s="6">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B54" s="9"/>
       <c r="C54" s="6"/>
@@ -1410,7 +1428,7 @@
     </row>
     <row r="55" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A55" s="6">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B55" s="9"/>
       <c r="C55" s="6"/>
@@ -1418,7 +1436,7 @@
     </row>
     <row r="56" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A56" s="6">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B56" s="9"/>
       <c r="C56" s="6"/>
@@ -1426,7 +1444,7 @@
     </row>
     <row r="57" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A57" s="6">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B57" s="9"/>
       <c r="C57" s="6"/>
@@ -1434,7 +1452,7 @@
     </row>
     <row r="58" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A58" s="6">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B58" s="9"/>
       <c r="C58" s="6"/>
@@ -1442,7 +1460,7 @@
     </row>
     <row r="59" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A59" s="6">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B59" s="9"/>
       <c r="C59" s="6"/>
@@ -1450,7 +1468,7 @@
     </row>
     <row r="60" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A60" s="6">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B60" s="9"/>
       <c r="C60" s="6"/>
@@ -1458,7 +1476,7 @@
     </row>
     <row r="61" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A61" s="6">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B61" s="9"/>
       <c r="C61" s="6"/>
@@ -1466,7 +1484,7 @@
     </row>
     <row r="62" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A62" s="6">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B62" s="9"/>
       <c r="C62" s="6"/>
@@ -1474,7 +1492,7 @@
     </row>
     <row r="63" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A63" s="6">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B63" s="9"/>
       <c r="C63" s="6"/>
@@ -1482,7 +1500,7 @@
     </row>
     <row r="64" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A64" s="6">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B64" s="9"/>
       <c r="C64" s="6"/>
@@ -1490,7 +1508,7 @@
     </row>
     <row r="65" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A65" s="6">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B65" s="9"/>
       <c r="C65" s="6"/>
@@ -1498,7 +1516,7 @@
     </row>
     <row r="66" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A66" s="6">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B66" s="9"/>
       <c r="C66" s="6"/>
@@ -1506,23 +1524,23 @@
     </row>
     <row r="67" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A67" s="6">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B67" s="9"/>
       <c r="C67" s="6"/>
-      <c r="D67" s="6"/>
+      <c r="D67" s="9"/>
     </row>
     <row r="68" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A68" s="6">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B68" s="9"/>
       <c r="C68" s="6"/>
-      <c r="D68" s="6"/>
+      <c r="D68" s="9"/>
     </row>
     <row r="69" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A69" s="6">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B69" s="9"/>
       <c r="C69" s="6"/>
@@ -1530,7 +1548,7 @@
     </row>
     <row r="70" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A70" s="6">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B70" s="9"/>
       <c r="C70" s="6"/>
@@ -1538,7 +1556,7 @@
     </row>
     <row r="71" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A71" s="6">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B71" s="9"/>
       <c r="C71" s="6"/>
@@ -1546,7 +1564,7 @@
     </row>
     <row r="72" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A72" s="6">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B72" s="9"/>
       <c r="C72" s="6"/>
@@ -1554,7 +1572,7 @@
     </row>
     <row r="73" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A73" s="6">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B73" s="9"/>
       <c r="C73" s="6"/>
@@ -1562,7 +1580,7 @@
     </row>
     <row r="74" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A74" s="6">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B74" s="9"/>
       <c r="C74" s="6"/>
@@ -1570,7 +1588,7 @@
     </row>
     <row r="75" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A75" s="6">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B75" s="9"/>
       <c r="C75" s="6"/>
@@ -1578,7 +1596,7 @@
     </row>
     <row r="76" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A76" s="6">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B76" s="9"/>
       <c r="C76" s="6"/>
@@ -1586,7 +1604,7 @@
     </row>
     <row r="77" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A77" s="6">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B77" s="9"/>
       <c r="C77" s="6"/>
@@ -1594,7 +1612,7 @@
     </row>
     <row r="78" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A78" s="6">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B78" s="9"/>
       <c r="C78" s="6"/>
@@ -1602,7 +1620,7 @@
     </row>
     <row r="79" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A79" s="6">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B79" s="9"/>
       <c r="C79" s="6"/>
@@ -1610,7 +1628,7 @@
     </row>
     <row r="80" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A80" s="6">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B80" s="9"/>
       <c r="C80" s="6"/>
@@ -1618,7 +1636,7 @@
     </row>
     <row r="81" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A81" s="6">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B81" s="9"/>
       <c r="C81" s="6"/>
@@ -1626,7 +1644,7 @@
     </row>
     <row r="82" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A82" s="6">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B82" s="9"/>
       <c r="C82" s="6"/>
@@ -1634,7 +1652,7 @@
     </row>
     <row r="83" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A83" s="6">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B83" s="9"/>
       <c r="C83" s="6"/>
@@ -1642,7 +1660,7 @@
     </row>
     <row r="84" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A84" s="6">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B84" s="9"/>
       <c r="C84" s="6"/>
@@ -1650,7 +1668,7 @@
     </row>
     <row r="85" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A85" s="6">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B85" s="9"/>
       <c r="C85" s="6"/>
@@ -1658,7 +1676,7 @@
     </row>
     <row r="86" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A86" s="6">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B86" s="9"/>
       <c r="C86" s="6"/>
@@ -1666,7 +1684,7 @@
     </row>
     <row r="87" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A87" s="6">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B87" s="9"/>
       <c r="C87" s="6"/>
@@ -1674,7 +1692,7 @@
     </row>
     <row r="88" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A88" s="6">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B88" s="9"/>
       <c r="C88" s="6"/>
@@ -1682,7 +1700,7 @@
     </row>
     <row r="89" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A89" s="6">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B89" s="9"/>
       <c r="C89" s="6"/>
@@ -1690,7 +1708,7 @@
     </row>
     <row r="90" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A90" s="6">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B90" s="9"/>
       <c r="C90" s="6"/>
@@ -1698,7 +1716,7 @@
     </row>
     <row r="91" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A91" s="6">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B91" s="9"/>
       <c r="C91" s="6"/>
@@ -1706,7 +1724,7 @@
     </row>
     <row r="92" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A92" s="6">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B92" s="9"/>
       <c r="C92" s="6"/>
@@ -1714,7 +1732,7 @@
     </row>
     <row r="93" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A93" s="6">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B93" s="9"/>
       <c r="C93" s="6"/>
@@ -1722,7 +1740,7 @@
     </row>
     <row r="94" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A94" s="6">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B94" s="9"/>
       <c r="C94" s="6"/>
@@ -1730,7 +1748,7 @@
     </row>
     <row r="95" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A95" s="6">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B95" s="9"/>
       <c r="C95" s="6"/>
@@ -1738,7 +1756,7 @@
     </row>
     <row r="96" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A96" s="6">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B96" s="9"/>
       <c r="C96" s="6"/>
@@ -1746,7 +1764,7 @@
     </row>
     <row r="97" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A97" s="6">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B97" s="9"/>
       <c r="C97" s="6"/>
@@ -1754,7 +1772,7 @@
     </row>
     <row r="98" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A98" s="6">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B98" s="9"/>
       <c r="C98" s="6"/>
@@ -1762,7 +1780,7 @@
     </row>
     <row r="99" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A99" s="6">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B99" s="9"/>
       <c r="C99" s="6"/>
@@ -1770,7 +1788,7 @@
     </row>
     <row r="100" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A100" s="6">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B100" s="9"/>
       <c r="C100" s="6"/>
@@ -1778,7 +1796,7 @@
     </row>
     <row r="101" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A101" s="6">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B101" s="9"/>
       <c r="C101" s="6"/>
@@ -1786,7 +1804,7 @@
     </row>
     <row r="102" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A102" s="6">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B102" s="9"/>
       <c r="C102" s="6"/>
@@ -1794,7 +1812,7 @@
     </row>
     <row r="103" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A103" s="6">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B103" s="9"/>
       <c r="C103" s="6"/>
@@ -1802,7 +1820,7 @@
     </row>
     <row r="104" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A104" s="6">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B104" s="9"/>
       <c r="C104" s="6"/>
@@ -1810,7 +1828,7 @@
     </row>
     <row r="105" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A105" s="6">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B105" s="9"/>
       <c r="C105" s="6"/>
@@ -1818,7 +1836,7 @@
     </row>
     <row r="106" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A106" s="6">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B106" s="9"/>
       <c r="C106" s="6"/>
@@ -1826,7 +1844,7 @@
     </row>
     <row r="107" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A107" s="6">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B107" s="9"/>
       <c r="C107" s="6"/>
@@ -1834,7 +1852,7 @@
     </row>
     <row r="108" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A108" s="6">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B108" s="9"/>
       <c r="C108" s="6"/>
@@ -1842,7 +1860,7 @@
     </row>
     <row r="109" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A109" s="6">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B109" s="9"/>
       <c r="C109" s="6"/>
@@ -1850,7 +1868,7 @@
     </row>
     <row r="110" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A110" s="6">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B110" s="9"/>
       <c r="C110" s="6"/>
@@ -1858,11 +1876,27 @@
     </row>
     <row r="111" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A111" s="6">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B111" s="9"/>
       <c r="C111" s="6"/>
       <c r="D111" s="6"/>
+    </row>
+    <row r="112" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A112" s="6">
+        <v>99</v>
+      </c>
+      <c r="B112" s="9"/>
+      <c r="C112" s="6"/>
+      <c r="D112" s="6"/>
+    </row>
+    <row r="113" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A113" s="6">
+        <v>100</v>
+      </c>
+      <c r="B113" s="9"/>
+      <c r="C113" s="6"/>
+      <c r="D113" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Completed Signup module with another test case and added HTML report
</commit_message>
<xml_diff>
--- a/resources/locators.xlsx
+++ b/resources/locators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaNi569\Desktop\CRMUIA\Generic_web_automation_framework\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C1E6B2-3173-4689-AE84-7B69F4F14F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25737A03-2604-40EF-BD3B-C8F52726AB92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32505" yWindow="1755" windowWidth="19185" windowHeight="10065" xr2:uid="{5EBB3FE3-55C9-4B90-8FD4-935120834B2F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5EBB3FE3-55C9-4B90-8FD4-935120834B2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="82">
   <si>
     <t>Page</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Locator type</t>
   </si>
   <si>
-    <t>Locator Value</t>
-  </si>
-  <si>
     <t>LoginPage</t>
   </si>
   <si>
@@ -282,6 +279,9 @@
   </si>
   <si>
     <t>Signup Button</t>
+  </si>
+  <si>
+    <t>Error Close Message</t>
   </si>
 </sst>
 </file>
@@ -722,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41983873-4B55-4713-B31B-EDCB84D265C4}">
-  <dimension ref="A1:D113"/>
+  <dimension ref="A1:D115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -747,616 +747,628 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>3</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>68</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B8" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>72</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:4" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>7</v>
-      </c>
       <c r="C14" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>16</v>
-      </c>
       <c r="C19" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B39" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="A41" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="8" t="s">
+    </row>
+    <row r="42" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="A42" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A40" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B40" s="8" t="s">
+      <c r="C42" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="6">
-        <v>31</v>
-      </c>
-      <c r="B44" s="9"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="9"/>
+      <c r="A44" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="45" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="6">
-        <v>32</v>
-      </c>
-      <c r="B45" s="9"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="9"/>
+      <c r="A45" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="46" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A46" s="6">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B46" s="9"/>
       <c r="C46" s="6"/>
@@ -1364,7 +1376,7 @@
     </row>
     <row r="47" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A47" s="6">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B47" s="9"/>
       <c r="C47" s="6"/>
@@ -1372,7 +1384,7 @@
     </row>
     <row r="48" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A48" s="6">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B48" s="9"/>
       <c r="C48" s="6"/>
@@ -1380,7 +1392,7 @@
     </row>
     <row r="49" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A49" s="6">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B49" s="9"/>
       <c r="C49" s="6"/>
@@ -1388,7 +1400,7 @@
     </row>
     <row r="50" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A50" s="6">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B50" s="9"/>
       <c r="C50" s="6"/>
@@ -1396,7 +1408,7 @@
     </row>
     <row r="51" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A51" s="6">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B51" s="9"/>
       <c r="C51" s="6"/>
@@ -1404,7 +1416,7 @@
     </row>
     <row r="52" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A52" s="6">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B52" s="9"/>
       <c r="C52" s="6"/>
@@ -1412,7 +1424,7 @@
     </row>
     <row r="53" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A53" s="6">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B53" s="9"/>
       <c r="C53" s="6"/>
@@ -1420,7 +1432,7 @@
     </row>
     <row r="54" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A54" s="6">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B54" s="9"/>
       <c r="C54" s="6"/>
@@ -1428,7 +1440,7 @@
     </row>
     <row r="55" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A55" s="6">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B55" s="9"/>
       <c r="C55" s="6"/>
@@ -1436,7 +1448,7 @@
     </row>
     <row r="56" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A56" s="6">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B56" s="9"/>
       <c r="C56" s="6"/>
@@ -1444,7 +1456,7 @@
     </row>
     <row r="57" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A57" s="6">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B57" s="9"/>
       <c r="C57" s="6"/>
@@ -1452,7 +1464,7 @@
     </row>
     <row r="58" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A58" s="6">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B58" s="9"/>
       <c r="C58" s="6"/>
@@ -1460,7 +1472,7 @@
     </row>
     <row r="59" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A59" s="6">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B59" s="9"/>
       <c r="C59" s="6"/>
@@ -1468,7 +1480,7 @@
     </row>
     <row r="60" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A60" s="6">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B60" s="9"/>
       <c r="C60" s="6"/>
@@ -1476,7 +1488,7 @@
     </row>
     <row r="61" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A61" s="6">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B61" s="9"/>
       <c r="C61" s="6"/>
@@ -1484,7 +1496,7 @@
     </row>
     <row r="62" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A62" s="6">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B62" s="9"/>
       <c r="C62" s="6"/>
@@ -1492,7 +1504,7 @@
     </row>
     <row r="63" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A63" s="6">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B63" s="9"/>
       <c r="C63" s="6"/>
@@ -1500,7 +1512,7 @@
     </row>
     <row r="64" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A64" s="6">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B64" s="9"/>
       <c r="C64" s="6"/>
@@ -1508,7 +1520,7 @@
     </row>
     <row r="65" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A65" s="6">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B65" s="9"/>
       <c r="C65" s="6"/>
@@ -1516,7 +1528,7 @@
     </row>
     <row r="66" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A66" s="6">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B66" s="9"/>
       <c r="C66" s="6"/>
@@ -1524,7 +1536,7 @@
     </row>
     <row r="67" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A67" s="6">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B67" s="9"/>
       <c r="C67" s="6"/>
@@ -1532,7 +1544,7 @@
     </row>
     <row r="68" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A68" s="6">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B68" s="9"/>
       <c r="C68" s="6"/>
@@ -1540,23 +1552,23 @@
     </row>
     <row r="69" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A69" s="6">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B69" s="9"/>
       <c r="C69" s="6"/>
-      <c r="D69" s="6"/>
+      <c r="D69" s="9"/>
     </row>
     <row r="70" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A70" s="6">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B70" s="9"/>
       <c r="C70" s="6"/>
-      <c r="D70" s="6"/>
+      <c r="D70" s="9"/>
     </row>
     <row r="71" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A71" s="6">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B71" s="9"/>
       <c r="C71" s="6"/>
@@ -1564,7 +1576,7 @@
     </row>
     <row r="72" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A72" s="6">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B72" s="9"/>
       <c r="C72" s="6"/>
@@ -1572,7 +1584,7 @@
     </row>
     <row r="73" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A73" s="6">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B73" s="9"/>
       <c r="C73" s="6"/>
@@ -1580,7 +1592,7 @@
     </row>
     <row r="74" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A74" s="6">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B74" s="9"/>
       <c r="C74" s="6"/>
@@ -1588,7 +1600,7 @@
     </row>
     <row r="75" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A75" s="6">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B75" s="9"/>
       <c r="C75" s="6"/>
@@ -1596,7 +1608,7 @@
     </row>
     <row r="76" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A76" s="6">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B76" s="9"/>
       <c r="C76" s="6"/>
@@ -1604,7 +1616,7 @@
     </row>
     <row r="77" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A77" s="6">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B77" s="9"/>
       <c r="C77" s="6"/>
@@ -1612,7 +1624,7 @@
     </row>
     <row r="78" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A78" s="6">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B78" s="9"/>
       <c r="C78" s="6"/>
@@ -1620,7 +1632,7 @@
     </row>
     <row r="79" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A79" s="6">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B79" s="9"/>
       <c r="C79" s="6"/>
@@ -1628,7 +1640,7 @@
     </row>
     <row r="80" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A80" s="6">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B80" s="9"/>
       <c r="C80" s="6"/>
@@ -1636,7 +1648,7 @@
     </row>
     <row r="81" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A81" s="6">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B81" s="9"/>
       <c r="C81" s="6"/>
@@ -1644,7 +1656,7 @@
     </row>
     <row r="82" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A82" s="6">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B82" s="9"/>
       <c r="C82" s="6"/>
@@ -1652,7 +1664,7 @@
     </row>
     <row r="83" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A83" s="6">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B83" s="9"/>
       <c r="C83" s="6"/>
@@ -1660,7 +1672,7 @@
     </row>
     <row r="84" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A84" s="6">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B84" s="9"/>
       <c r="C84" s="6"/>
@@ -1668,7 +1680,7 @@
     </row>
     <row r="85" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A85" s="6">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B85" s="9"/>
       <c r="C85" s="6"/>
@@ -1676,7 +1688,7 @@
     </row>
     <row r="86" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A86" s="6">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B86" s="9"/>
       <c r="C86" s="6"/>
@@ -1684,7 +1696,7 @@
     </row>
     <row r="87" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A87" s="6">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B87" s="9"/>
       <c r="C87" s="6"/>
@@ -1692,7 +1704,7 @@
     </row>
     <row r="88" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A88" s="6">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B88" s="9"/>
       <c r="C88" s="6"/>
@@ -1700,7 +1712,7 @@
     </row>
     <row r="89" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A89" s="6">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B89" s="9"/>
       <c r="C89" s="6"/>
@@ -1708,7 +1720,7 @@
     </row>
     <row r="90" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A90" s="6">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B90" s="9"/>
       <c r="C90" s="6"/>
@@ -1716,7 +1728,7 @@
     </row>
     <row r="91" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A91" s="6">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B91" s="9"/>
       <c r="C91" s="6"/>
@@ -1724,7 +1736,7 @@
     </row>
     <row r="92" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A92" s="6">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B92" s="9"/>
       <c r="C92" s="6"/>
@@ -1732,7 +1744,7 @@
     </row>
     <row r="93" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A93" s="6">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B93" s="9"/>
       <c r="C93" s="6"/>
@@ -1740,7 +1752,7 @@
     </row>
     <row r="94" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A94" s="6">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B94" s="9"/>
       <c r="C94" s="6"/>
@@ -1748,7 +1760,7 @@
     </row>
     <row r="95" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A95" s="6">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B95" s="9"/>
       <c r="C95" s="6"/>
@@ -1756,7 +1768,7 @@
     </row>
     <row r="96" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A96" s="6">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B96" s="9"/>
       <c r="C96" s="6"/>
@@ -1764,7 +1776,7 @@
     </row>
     <row r="97" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A97" s="6">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B97" s="9"/>
       <c r="C97" s="6"/>
@@ -1772,7 +1784,7 @@
     </row>
     <row r="98" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A98" s="6">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B98" s="9"/>
       <c r="C98" s="6"/>
@@ -1780,7 +1792,7 @@
     </row>
     <row r="99" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A99" s="6">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B99" s="9"/>
       <c r="C99" s="6"/>
@@ -1788,7 +1800,7 @@
     </row>
     <row r="100" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A100" s="6">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B100" s="9"/>
       <c r="C100" s="6"/>
@@ -1796,7 +1808,7 @@
     </row>
     <row r="101" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A101" s="6">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B101" s="9"/>
       <c r="C101" s="6"/>
@@ -1804,7 +1816,7 @@
     </row>
     <row r="102" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A102" s="6">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B102" s="9"/>
       <c r="C102" s="6"/>
@@ -1812,7 +1824,7 @@
     </row>
     <row r="103" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A103" s="6">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B103" s="9"/>
       <c r="C103" s="6"/>
@@ -1820,7 +1832,7 @@
     </row>
     <row r="104" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A104" s="6">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B104" s="9"/>
       <c r="C104" s="6"/>
@@ -1828,7 +1840,7 @@
     </row>
     <row r="105" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A105" s="6">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B105" s="9"/>
       <c r="C105" s="6"/>
@@ -1836,7 +1848,7 @@
     </row>
     <row r="106" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A106" s="6">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B106" s="9"/>
       <c r="C106" s="6"/>
@@ -1844,7 +1856,7 @@
     </row>
     <row r="107" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A107" s="6">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B107" s="9"/>
       <c r="C107" s="6"/>
@@ -1852,7 +1864,7 @@
     </row>
     <row r="108" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A108" s="6">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B108" s="9"/>
       <c r="C108" s="6"/>
@@ -1860,7 +1872,7 @@
     </row>
     <row r="109" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A109" s="6">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B109" s="9"/>
       <c r="C109" s="6"/>
@@ -1868,7 +1880,7 @@
     </row>
     <row r="110" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A110" s="6">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B110" s="9"/>
       <c r="C110" s="6"/>
@@ -1876,7 +1888,7 @@
     </row>
     <row r="111" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A111" s="6">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B111" s="9"/>
       <c r="C111" s="6"/>
@@ -1884,7 +1896,7 @@
     </row>
     <row r="112" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A112" s="6">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B112" s="9"/>
       <c r="C112" s="6"/>
@@ -1892,11 +1904,27 @@
     </row>
     <row r="113" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A113" s="6">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B113" s="9"/>
       <c r="C113" s="6"/>
       <c r="D113" s="6"/>
+    </row>
+    <row r="114" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A114" s="6">
+        <v>99</v>
+      </c>
+      <c r="B114" s="9"/>
+      <c r="C114" s="6"/>
+      <c r="D114" s="6"/>
+    </row>
+    <row r="115" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A115" s="6">
+        <v>100</v>
+      </c>
+      <c r="B115" s="9"/>
+      <c r="C115" s="6"/>
+      <c r="D115" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>